<commit_message>
[EXTRA SCRAPE] full data scraped for extra batting and bowling fields
</commit_message>
<xml_diff>
--- a/bin/sheets/main_db/active_players/all_formats/ActivePlayers_NZL.xlsx
+++ b/bin/sheets/main_db/active_players/all_formats/ActivePlayers_NZL.xlsx
@@ -579,7 +579,7 @@
         <v>2</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
@@ -640,7 +640,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11">
@@ -783,7 +783,7 @@
         <v>67</v>
       </c>
       <c r="E17" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18">
@@ -846,7 +846,7 @@
         <v>125</v>
       </c>
       <c r="E20" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21">
@@ -863,7 +863,7 @@
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22">
@@ -899,7 +899,7 @@
         <v>42</v>
       </c>
       <c r="E23" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24">
@@ -920,7 +920,7 @@
         <v>21</v>
       </c>
       <c r="E24" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25">
@@ -941,7 +941,7 @@
         <v>71</v>
       </c>
       <c r="E25" t="n">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26">
@@ -1023,7 +1023,7 @@
         <v>2</v>
       </c>
       <c r="E29" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30">
@@ -1099,7 +1099,7 @@
         <v>3</v>
       </c>
       <c r="E33" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34">
@@ -1139,7 +1139,7 @@
         <v>41</v>
       </c>
       <c r="E35" t="n">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36">

</xml_diff>